<commit_message>
Added Power Button Control Circuit
</commit_message>
<xml_diff>
--- a/CM4/bom.xlsx
+++ b/CM4/bom.xlsx
@@ -46,10 +46,10 @@
     <t xml:space="preserve">TPS61230DRCR </t>
   </si>
   <si>
-    <t xml:space="preserve">TPS61232DRC </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MUST HAVE FIXED 5V out</t>
+    <t xml:space="preserve">Power Control Tranistor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/goford-semiconductor/G6N02L/13664832</t>
   </si>
 </sst>
 </file>
@@ -167,10 +167,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
+      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -219,11 +219,16 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removed Keyboard Matrix Diodes and Added PowerLED and ActivityLED
</commit_message>
<xml_diff>
--- a/CM4/bom.xlsx
+++ b/CM4/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hailey\Desktop\Current ti92Project\TI92-revive-main\TI92-RPI-Zero\CM4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086B4B5D-2C80-4333-82CE-0E6B21E718A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE9015C-EB90-498A-8F48-FE1881F3D4C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>B2B-PH-K-S(LF)(SN)</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>TQ2SA-L2-3V</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/stewart-connector/SS-52100-001/7902377</t>
   </si>
 </sst>
 </file>
@@ -438,7 +441,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,8 +499,13 @@
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="A17" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -509,8 +517,9 @@
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" display="TPS61230DRCR" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A22" r:id="rId2" display="https://www.mouser.com/ProductDetail/Panasonic-Industrial-Devices/TQ2SA-L2-3V?qs=UO%2Fx91QLkSDLsw6acU2Ugw%3D%3D" xr:uid="{87E714EF-B81C-41ED-BAED-F46E1609C932}"/>
+    <hyperlink ref="A17" r:id="rId3" xr:uid="{12AC56B9-A9A6-4FDB-A484-825C71C68AF3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finally Added the display!!!!
</commit_message>
<xml_diff>
--- a/CM4/bom.xlsx
+++ b/CM4/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">B2B-PH-K-S(LF)(SN)</t>
   </si>
@@ -82,7 +82,13 @@
     <t xml:space="preserve">Crystle</t>
   </si>
   <si>
+    <t xml:space="preserve">The display</t>
+  </si>
+  <si>
     <t xml:space="preserve">1v regulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.waveshare.com/4inch-RPi-LCD-C.htm</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/TLV74010PDBVR/12642176</t>
@@ -293,10 +299,10 @@
   <dimension ref="A1:R30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N26" activeCellId="0" sqref="N26"/>
+      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -314,12 +320,12 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -338,7 +344,7 @@
       <c r="A11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P12" s="0" t="s">
+      <c r="P12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -346,7 +352,7 @@
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="P13" s="0" t="s">
+      <c r="P13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
@@ -354,7 +360,7 @@
       <c r="A14" s="3"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -364,12 +370,12 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P18" s="0" t="s">
+      <c r="P18" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="21.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>13</v>
       </c>
       <c r="P19" s="5" t="s">
@@ -377,7 +383,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P21" s="0" t="s">
+      <c r="P21" s="1" t="s">
         <v>15</v>
       </c>
     </row>
@@ -390,23 +396,29 @@
       <c r="P26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="R26" s="0" t="s">
+      <c r="R26" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="R27" s="0" t="s">
+      <c r="R27" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P29" s="0" t="s">
+      <c r="C29" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="P29" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="P30" s="0" t="s">
-        <v>21</v>
+      <c r="C30" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="P30" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bigone here we go
Whats gonna happon is im gonna get a 4 inch hdmi display and desolder the hdmi connector and add it to a ribbion cable and then add a connector to the pcb for hdmi to interface with that
</commit_message>
<xml_diff>
--- a/CM4/bom.xlsx
+++ b/CM4/bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t xml:space="preserve">B2B-PH-K-S(LF)(SN)</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.com/en/products/detail/texas-instruments/TLV74010PDBVR/12642176</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.com/en/products/detail/delta-electronics/BSB0205HP-00EFG/11201159?s=N4IgTCBcDaIEIGU4AYzIKwAkAKBaZyAogGIDiIAugL5A</t>
   </si>
 </sst>
 </file>
@@ -296,13 +302,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R30"/>
+  <dimension ref="A1:R35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B34" activeCellId="0" sqref="B34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -406,7 +412,7 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="P29" s="1" t="s">
@@ -414,11 +420,21 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>22</v>
       </c>
       <c r="P30" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>